<commit_message>
add README and LICENSE files; add documentations and comments to codebase
</commit_message>
<xml_diff>
--- a/figures/ft/selected.xlsx
+++ b/figures/ft/selected.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -468,15 +468,15 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{thumb, index} (distance) {diff} - |spectral| rel_pwr_2_to_4</t>
+          <t>{thumb, index} (distance) {diff} - |spectral| entropy</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -484,17 +484,33 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{thumb, index} (distance) {diff} - |temporal| mad</t>
+          <t>{thumb, index} (distance) {diff} - |spectral| rel_pwr_2_to_4</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>{thumb, index} (distance) {diff} - |temporal| mad</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>